<commit_message>
merged to protocol sg
</commit_message>
<xml_diff>
--- a/src/main/resources/ru/avem/kspem/app/protocolDPT.xlsx
+++ b/src/main/resources/ru/avem/kspem/app/protocolDPT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="112">
   <si>
     <t xml:space="preserve">г. Новочеркасск</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">#date#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#time#</t>
   </si>
   <si>
     <t xml:space="preserve">Номинальные параметры объекта испытания</t>
@@ -915,11 +918,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A28" colorId="64" zoomScale="85" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="17.71"/>
@@ -1122,7 +1125,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J12" s="21"/>
       <c r="K12" s="22"/>
@@ -1159,7 +1162,7 @@
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="26"/>
       <c r="B14" s="27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -1293,25 +1296,25 @@
     <row r="16" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="30"/>
       <c r="B16" s="25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" s="25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H16" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="35"/>
@@ -1373,25 +1376,25 @@
     <row r="17" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="30"/>
       <c r="B17" s="25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I17" s="34"/>
       <c r="J17" s="35"/>
@@ -1585,7 +1588,7 @@
     <row r="20" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="26"/>
       <c r="B20" s="40" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -1720,22 +1723,22 @@
       <c r="A22" s="30"/>
       <c r="B22" s="0"/>
       <c r="C22" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D22" s="42" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F22" s="42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H22" s="43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I22" s="43"/>
       <c r="J22" s="34"/>
@@ -1797,25 +1800,25 @@
     <row r="23" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="30"/>
       <c r="B23" s="25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" s="42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F23" s="42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G23" s="42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H23" s="44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I23" s="44"/>
       <c r="J23" s="34"/>
@@ -1877,25 +1880,25 @@
     <row r="24" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="30"/>
       <c r="B24" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" s="42" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F24" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H24" s="44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I24" s="44"/>
       <c r="J24" s="35"/>
@@ -1957,25 +1960,25 @@
     <row r="25" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="30"/>
       <c r="B25" s="25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F25" s="42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H25" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="35"/>
@@ -2169,7 +2172,7 @@
     <row r="28" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="26"/>
       <c r="B28" s="40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C28" s="40"/>
       <c r="D28" s="40"/>
@@ -2303,18 +2306,18 @@
     <row r="30" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="30"/>
       <c r="B30" s="25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C30" s="25"/>
       <c r="D30" s="25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E30" s="25"/>
       <c r="F30" s="45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G30" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H30" s="45"/>
       <c r="I30" s="34"/>
@@ -2377,18 +2380,18 @@
     <row r="31" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="30"/>
       <c r="B31" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" s="25"/>
       <c r="D31" s="25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E31" s="25"/>
       <c r="F31" s="25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G31" s="25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H31" s="25"/>
       <c r="I31" s="34"/>
@@ -2583,7 +2586,7 @@
     <row r="34" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="26"/>
       <c r="B34" s="40" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C34" s="40"/>
       <c r="D34" s="40"/>
@@ -2717,17 +2720,17 @@
     <row r="36" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="30"/>
       <c r="B36" s="25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
       <c r="H36" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I36" s="25"/>
       <c r="J36" s="35"/>
@@ -2789,17 +2792,17 @@
     <row r="37" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="30"/>
       <c r="B37" s="25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
       <c r="E37" s="25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
       <c r="H37" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I37" s="25"/>
       <c r="J37" s="35"/>
@@ -2993,7 +2996,7 @@
     <row r="40" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="26"/>
       <c r="B40" s="27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
@@ -3128,19 +3131,19 @@
       <c r="A42" s="30"/>
       <c r="B42" s="34"/>
       <c r="C42" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E42" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G42" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -3204,19 +3207,19 @@
       <c r="A43" s="30"/>
       <c r="B43" s="34"/>
       <c r="C43" s="25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D43" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
@@ -3346,19 +3349,19 @@
       <c r="A45" s="30"/>
       <c r="B45" s="34"/>
       <c r="C45" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G45" s="43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H45" s="34"/>
       <c r="I45" s="34"/>
@@ -3422,19 +3425,19 @@
       <c r="A46" s="30"/>
       <c r="B46" s="34"/>
       <c r="C46" s="25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G46" s="44" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
@@ -3629,7 +3632,7 @@
     <row r="49" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="26"/>
       <c r="B49" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
@@ -3764,19 +3767,19 @@
       <c r="A51" s="30"/>
       <c r="B51" s="34"/>
       <c r="C51" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E51" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F51" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G51" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H51" s="34"/>
       <c r="I51" s="34"/>
@@ -3840,19 +3843,19 @@
       <c r="A52" s="30"/>
       <c r="B52" s="34"/>
       <c r="C52" s="25" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D52" s="25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F52" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G52" s="25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
@@ -3982,19 +3985,19 @@
       <c r="A54" s="30"/>
       <c r="B54" s="34"/>
       <c r="C54" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D54" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G54" s="43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H54" s="34"/>
       <c r="I54" s="34"/>
@@ -4058,19 +4061,19 @@
       <c r="A55" s="30"/>
       <c r="B55" s="34"/>
       <c r="C55" s="25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H55" s="34"/>
       <c r="I55" s="34"/>
@@ -4265,7 +4268,7 @@
     <row r="58" customFormat="false" ht="20.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="26"/>
       <c r="B58" s="27" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C58" s="27"/>
       <c r="D58" s="27"/>
@@ -4400,19 +4403,19 @@
       <c r="A60" s="30"/>
       <c r="B60" s="34"/>
       <c r="C60" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D60" s="25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G60" s="25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H60" s="34"/>
       <c r="I60" s="34"/>
@@ -4476,19 +4479,19 @@
       <c r="A61" s="30"/>
       <c r="B61" s="34"/>
       <c r="C61" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G61" s="25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H61" s="34"/>
       <c r="I61" s="34"/>
@@ -4618,19 +4621,19 @@
       <c r="A63" s="30"/>
       <c r="B63" s="34"/>
       <c r="C63" s="25" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D63" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G63" s="43" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H63" s="34"/>
       <c r="I63" s="34"/>
@@ -4648,19 +4651,19 @@
       <c r="A64" s="30"/>
       <c r="B64" s="34"/>
       <c r="C64" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D64" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F64" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G64" s="44" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H64" s="34"/>
       <c r="I64" s="34"/>
@@ -4737,7 +4740,7 @@
     <row r="68" s="23" customFormat="true" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
       <c r="B68" s="49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C68" s="49"/>
       <c r="D68" s="50"/>
@@ -4844,19 +4847,19 @@
     <row r="73" s="23" customFormat="true" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
       <c r="B73" s="52" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C73" s="52"/>
       <c r="D73" s="53" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E73" s="53"/>
       <c r="F73" s="54"/>
       <c r="G73" s="52" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H73" s="50" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I73" s="50"/>
       <c r="J73" s="49"/>
@@ -4923,7 +4926,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.590277777777778" top="0.590277777777778" bottom="0.590277777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="51" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="51" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
protocol AIEL ZavNomer i logo
</commit_message>
<xml_diff>
--- a/src/main/resources/ru/avem/kspem/app/protocolDPT.xlsx
+++ b/src/main/resources/ru/avem/kspem/app/protocolDPT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t xml:space="preserve">г. Новочеркасск</t>
   </si>
@@ -356,6 +356,24 @@
   </si>
   <si>
     <t xml:space="preserve">#date# </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Степень искрения коммутации при номинальной нагрузке и кратковременной перезгрузке по току</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точка 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точка 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точка 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точка 4</t>
   </si>
 </sst>
 </file>
@@ -500,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -592,6 +610,13 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -618,7 +643,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -837,6 +862,10 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -916,13 +945,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ73"/>
+  <dimension ref="A1:AMJ78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A58" colorId="64" zoomScale="85" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M81" activeCellId="0" sqref="M81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="1" width="17.71"/>
@@ -4873,8 +4902,46 @@
       <c r="AMI73" s="0"/>
       <c r="AMJ73" s="0"/>
     </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="0"/>
+      <c r="C75" s="0"/>
+      <c r="D75" s="0"/>
+      <c r="E75" s="0"/>
+      <c r="F75" s="0"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0"/>
+    </row>
+    <row r="77" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C77" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D77" s="55"/>
+      <c r="E77" s="55"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0"/>
+      <c r="C78" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E78" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F78" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="G78" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="H78" s="0"/>
+    </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="49">
     <mergeCell ref="A1:C6"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:I1"/>
@@ -4923,10 +4990,11 @@
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:E73"/>
     <mergeCell ref="H73:I73"/>
+    <mergeCell ref="C77:G77"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.590277777777778" top="0.590277777777778" bottom="0.590277777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="51" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="51" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>